<commit_message>
Doc: Informe de incidencia y de riesgos terminados
</commit_message>
<xml_diff>
--- a/Recursos/Informes Vesta/Informe de seguimiento.xlsx
+++ b/Recursos/Informes Vesta/Informe de seguimiento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cintia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cintia\Desktop\Cintia\Uni\Regular\Laboratorio de desarrollo de software\Vesta_Risk_Manager\Recursos\Informes Vesta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980D426B-D7E3-4469-9B70-FF22F065F988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77D9DAD-9F0D-41F8-BC83-060AF2596C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{0B7A402A-43A1-4A95-8AAE-5FC7A7913B98}"/>
   </bookViews>
@@ -18,17 +18,28 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>PLANTILLA DE SEGUIMIENTO DE RIESGOS</t>
   </si>
@@ -81,12 +92,6 @@
     <t>PRIORIDAD</t>
   </si>
   <si>
-    <t>ASIGNADO</t>
-  </si>
-  <si>
-    <t>ABIERTO</t>
-  </si>
-  <si>
     <t>COMENTARIOS</t>
   </si>
   <si>
@@ -119,6 +124,9 @@
   <si>
     <t>El socio no se presentó</t>
   </si>
+  <si>
+    <t>RESPONSABLE</t>
+  </si>
 </sst>
 </file>
 
@@ -128,9 +136,9 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;XDR&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +176,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Century Gothic"/>
       <family val="1"/>
     </font>
@@ -261,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -313,17 +328,22 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -580,7 +600,6 @@
           </c:dPt>
           <c:dLbls>
             <c:delete val="1"/>
-            <c:extLst/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2186,13 +2205,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>53975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2224,13 +2243,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>768350</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2256,6 +2275,117 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>84937</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>159264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1" descr="Institucional - Portal UNPA UARG">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{432984FC-C639-614C-AC22-613F412F5BBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="84937" y="159264"/>
+          <a:ext cx="515138" cy="755136"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>257174</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AAB545A-7A5B-12ED-A897-FE3DF8318BC6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="514351" y="238125"/>
+          <a:ext cx="1019174" cy="1019174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2317,8 +2447,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2621,10 +2751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07C9C91-ECE1-41D5-B84F-19E079D652A8}">
-  <dimension ref="A1:AA51"/>
+  <dimension ref="A1:AA53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,13 +2765,13 @@
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="44.140625" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -2666,31 +2796,22 @@
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
     </row>
-    <row r="2" spans="1:27" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>6</v>
-      </c>
+    <row r="2" spans="1:27" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="J2" s="13"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+      <c r="N2" s="13"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -2705,33 +2826,20 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
     </row>
-    <row r="3" spans="1:27" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="10">
-        <f>COUNTIF($D$21:$D$32,E3)</f>
-        <v>2</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="12">
-        <f>COUNTIF($E$21:$E$32,G3)</f>
-        <v>4</v>
-      </c>
+    <row r="3" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="J3" s="13"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="N3" s="13"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -2746,28 +2854,26 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
     </row>
-    <row r="4" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="10">
-        <f>COUNTIF($D$21:$D$32,E4)</f>
-        <v>3</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="12">
-        <f>COUNTIF($E$21:$E$32,G4)</f>
-        <v>3</v>
-      </c>
-      <c r="I4" s="5"/>
+      <c r="E4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -2775,7 +2881,7 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
-      <c r="Q4" s="13"/>
+      <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -2787,28 +2893,28 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
     </row>
-    <row r="5" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="5"/>
       <c r="E5" s="9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F5" s="10">
-        <f>COUNTIF($D$21:$D$32,E5)</f>
-        <v>5</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="12">
-        <f>COUNTIF($E$21:$E$32,G5)</f>
-        <v>3</v>
-      </c>
-      <c r="I5" s="13"/>
+        <f>COUNTIF($D$23:$D$34,E5)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="12">
+        <f>COUNTIF($E$23:$E$34,H5)</f>
+        <v>4</v>
+      </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -2817,32 +2923,47 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
-      <c r="R5" s="13"/>
+      <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-      <c r="V5" s="13"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
     </row>
-    <row r="6" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="5"/>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="5"/>
-      <c r="F6" s="13"/>
+      <c r="E6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10">
+        <f>COUNTIF($D$23:$D$34,E6)</f>
+        <v>3</v>
+      </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="13"/>
+      <c r="H6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="12">
+        <f>COUNTIF($E$23:$E$34,H6)</f>
+        <v>3</v>
+      </c>
+      <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-      <c r="N6" s="13"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="Q6" s="13"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
@@ -2854,16 +2975,28 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
     </row>
-    <row r="7" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="10">
+        <f>COUNTIF($D$23:$D$34,E7)</f>
+        <v>5</v>
+      </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="H7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="12">
+        <f>COUNTIF($E$23:$E$34,H7)</f>
+        <v>3</v>
+      </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -2872,11 +3005,10 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
+      <c r="R7" s="13"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
+      <c r="V7" s="13"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
@@ -2885,19 +3017,17 @@
     </row>
     <row r="8" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="J8" s="13"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="N8" s="13"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
@@ -2921,7 +3051,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="13"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -2942,7 +3072,7 @@
       <c r="AA9" s="5"/>
     </row>
     <row r="10" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2951,13 +3081,14 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="13"/>
+      <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
-      <c r="N10" s="13"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-      <c r="Q10" s="13"/>
+      <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
@@ -2971,13 +3102,14 @@
     </row>
     <row r="11" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -2986,10 +3118,11 @@
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
-      <c r="R11" s="13"/>
+      <c r="R11" s="5"/>
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
-      <c r="V11" s="13"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
@@ -2997,7 +3130,7 @@
       <c r="AA11" s="5"/>
     </row>
     <row r="12" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -3006,14 +3139,13 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
+      <c r="N12" s="13"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
+      <c r="Q12" s="13"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
@@ -3027,11 +3159,10 @@
     </row>
     <row r="13" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -3043,11 +3174,10 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
+      <c r="R13" s="13"/>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
+      <c r="V13" s="13"/>
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
@@ -3084,7 +3214,7 @@
       <c r="AA14" s="5"/>
     </row>
     <row r="15" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -3092,7 +3222,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="13"/>
+      <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -3114,20 +3244,22 @@
     </row>
     <row r="16" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="13"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="F16" s="13"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="13"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="N16" s="13"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
-      <c r="Q16" s="13"/>
+      <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
@@ -3140,7 +3272,7 @@
       <c r="AA16" s="5"/>
     </row>
     <row r="17" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -3148,7 +3280,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="I17" s="13"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -3157,10 +3289,11 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
-      <c r="R17" s="13"/>
+      <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
-      <c r="V17" s="13"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
       <c r="W17" s="5"/>
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
@@ -3169,22 +3302,20 @@
     </row>
     <row r="18" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="J18" s="13"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
+      <c r="N18" s="13"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
+      <c r="Q18" s="13"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
@@ -3214,43 +3345,26 @@
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
+      <c r="R19" s="13"/>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
+      <c r="V19" s="13"/>
       <c r="W19" s="5"/>
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
@@ -3259,34 +3373,27 @@
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
-      <c r="R20" s="13"/>
+      <c r="R20" s="5"/>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
-      <c r="V20" s="13"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
       <c r="W20" s="5"/>
       <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
       <c r="Z20" s="5"/>
       <c r="AA20" s="5"/>
     </row>
-    <row r="21" spans="1:27" ht="27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="15">
-        <v>1</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="18"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -3308,22 +3415,26 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="15">
-        <v>2</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="18"/>
+      <c r="B22" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="18"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -3332,35 +3443,34 @@
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
+      <c r="R22" s="13"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
-      <c r="V22" s="5"/>
+      <c r="V22" s="13"/>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
     </row>
-    <row r="23" spans="1:27" ht="27" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
       <c r="B23" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F23" s="16"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="18"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -3383,21 +3493,21 @@
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="18"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -3406,7 +3516,7 @@
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
-      <c r="R24" s="13"/>
+      <c r="R24" s="5"/>
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
@@ -3418,24 +3528,24 @@
       <c r="AA24" s="5"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E25" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="16"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="13"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
@@ -3444,10 +3554,11 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
-      <c r="S25" s="13"/>
+      <c r="S25" s="5"/>
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
-      <c r="W25" s="13"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
@@ -3456,29 +3567,30 @@
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F26" s="16"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="18"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="13"/>
+      <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
-      <c r="O26" s="13"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
+      <c r="R26" s="13"/>
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
@@ -3489,25 +3601,25 @@
       <c r="Z26" s="5"/>
       <c r="AA26" s="5"/>
     </row>
-    <row r="27" spans="1:27" ht="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="16"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="5"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="13"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
@@ -3515,39 +3627,39 @@
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
-      <c r="S27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="13"/>
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
+      <c r="W27" s="13"/>
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
-    </row>
-    <row r="28" spans="1:27" ht="27" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
+      <c r="AA27" s="5"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
       <c r="B28" s="15">
+        <v>6</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>10</v>
-      </c>
       <c r="F28" s="16"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="18"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="13"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
+      <c r="K28" s="13"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
+      <c r="O28" s="13"/>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
@@ -3564,21 +3676,21 @@
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="15">
+        <v>7</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>11</v>
-      </c>
       <c r="E29" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F29" s="16"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="18"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
@@ -3587,7 +3699,6 @@
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
@@ -3596,26 +3707,25 @@
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
-    </row>
-    <row r="30" spans="1:27" ht="27" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
       <c r="B30" s="15">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E30" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F30" s="16"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="18"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
@@ -3637,13 +3747,21 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="B31" s="15">
+        <v>9</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="16"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -3666,13 +3784,21 @@
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="B32" s="15">
+        <v>10</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="16"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="20"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
@@ -3723,7 +3849,7 @@
       <c r="AA33" s="5"/>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
+      <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -3753,10 +3879,11 @@
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" s="13"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="F35" s="13"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -3780,7 +3907,7 @@
       <c r="AA35" s="5"/>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
+      <c r="A36" s="13"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -3810,11 +3937,10 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="F37" s="13"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -3867,7 +3993,7 @@
       <c r="AA38" s="5"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
+      <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -3897,10 +4023,11 @@
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="13"/>
+      <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="F40" s="13"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -3924,7 +4051,7 @@
       <c r="AA40" s="5"/>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
+      <c r="A41" s="13"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -3954,11 +4081,10 @@
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
+      <c r="F42" s="13"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -4011,7 +4137,7 @@
       <c r="AA43" s="5"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
+      <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -4041,10 +4167,11 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
-      <c r="B45" s="13"/>
+      <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
-      <c r="F45" s="13"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -4068,7 +4195,7 @@
       <c r="AA45" s="5"/>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
+      <c r="A46" s="13"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -4098,11 +4225,10 @@
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
+      <c r="F47" s="13"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -4155,7 +4281,7 @@
       <c r="AA48" s="5"/>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
+      <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -4185,10 +4311,11 @@
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
-      <c r="B50" s="13"/>
+      <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
-      <c r="F50" s="13"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
@@ -4212,7 +4339,7 @@
       <c r="AA50" s="5"/>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
+      <c r="A51" s="13"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -4240,7 +4367,77 @@
       <c r="Z51" s="5"/>
       <c r="AA51" s="5"/>
     </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5"/>
+      <c r="T52" s="5"/>
+      <c r="U52" s="5"/>
+      <c r="V52" s="5"/>
+      <c r="W52" s="5"/>
+      <c r="X52" s="5"/>
+      <c r="Y52" s="5"/>
+      <c r="Z52" s="5"/>
+      <c r="AA52" s="5"/>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="5"/>
+      <c r="Y53" s="5"/>
+      <c r="Z53" s="5"/>
+      <c r="AA53" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G27:H27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>